<commit_message>
modif 2 de pagos sobre saldo
</commit_message>
<xml_diff>
--- a/Calculos.xlsx
+++ b/Calculos.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Pagos</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Totales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deuda </t>
   </si>
 </sst>
 </file>
@@ -719,10 +722,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H17"/>
+  <dimension ref="B3:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,7 +733,7 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>1</v>
       </c>
@@ -738,7 +741,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>2</v>
       </c>
@@ -746,7 +749,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>11</v>
       </c>
@@ -754,7 +757,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -774,7 +777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>44257</v>
       </c>
@@ -800,7 +803,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>44288</v>
       </c>
@@ -808,7 +811,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="2">
-        <f>$D$7-E8</f>
+        <f>D7-E8</f>
         <v>27850</v>
       </c>
       <c r="E8" s="2">
@@ -826,7 +829,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>44318</v>
       </c>
@@ -834,8 +837,8 @@
         <v>3</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" ref="D9:D10" si="1">$D$7-E9</f>
-        <v>34000</v>
+        <f t="shared" ref="D9:D10" si="1">D8-E9</f>
+        <v>27850</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -844,15 +847,15 @@
         <v>0</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="0"/>
+        <f>E9+F9</f>
         <v>0</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" ref="H9:H10" si="2">D8*$E$4/100/12</f>
+        <f t="shared" ref="H9:H11" si="2">D8*$E$4/100/12</f>
         <v>696.25</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>44349</v>
       </c>
@@ -861,20 +864,24 @@
       </c>
       <c r="D10" s="2">
         <f t="shared" si="1"/>
-        <v>34000</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+        <v>22242.5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5607.5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1392.5</v>
+      </c>
       <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>E10+F10</f>
+        <v>7000</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="2"/>
-        <v>850</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+        <v>696.25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>44379</v>
       </c>
@@ -888,9 +895,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="2">
+        <f t="shared" si="2"/>
+        <v>556.0625</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>44410</v>
       </c>
@@ -905,7 +915,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>44441</v>
       </c>
@@ -920,7 +930,7 @@
       </c>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>44471</v>
       </c>
@@ -935,7 +945,7 @@
       </c>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>44502</v>
       </c>
@@ -950,7 +960,7 @@
       </c>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>44532</v>
       </c>
@@ -963,26 +973,39 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="2">
         <f>SUM(D7:D10)</f>
-        <v>129850</v>
+        <v>111942.5</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" ref="E17:H17" si="3">SUM(E7:E10)</f>
-        <v>12150</v>
+        <v>17757.5</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="3"/>
-        <v>1850</v>
+        <v>3242.5</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="3"/>
-        <v>3396.25</v>
+        <v>3242.5</v>
+      </c>
+      <c r="I17" s="2">
+        <f>H17-F17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="2">
+        <f>H17-H7-H8-H9-H11</f>
+        <v>140.1875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios a medias de interes periodo
</commit_message>
<xml_diff>
--- a/Calculos.xlsx
+++ b/Calculos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -391,8 +391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +475,7 @@
       </c>
       <c r="K5" s="2">
         <f>($D$2-SUM($D$5:D8))*30/100/12</f>
-        <v>1491.1699999999994</v>
+        <v>1433.3184999999996</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -509,7 +509,7 @@
       </c>
       <c r="K6" s="2">
         <f>($D$2-SUM($D$5:D9))*30/100/12</f>
-        <v>1331.7949999999996</v>
+        <v>1244.1514999999997</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -521,13 +521,13 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ref="C7:C9" si="2">C6-D7</f>
-        <v>65996.87999999999</v>
+        <v>63739.259999999995</v>
       </c>
       <c r="D7" s="2">
-        <v>13748.74</v>
+        <v>16006.36</v>
       </c>
       <c r="E7" s="2">
-        <v>4251.26</v>
+        <v>1993.64</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
@@ -543,7 +543,7 @@
       </c>
       <c r="K7" s="2">
         <f>($D$2-SUM($D$5:D10))*30/100/12</f>
-        <v>1331.7949999999996</v>
+        <v>900.25524999999982</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -555,13 +555,13 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" si="2"/>
-        <v>59646.799999999988</v>
+        <v>57332.739999999991</v>
       </c>
       <c r="D8" s="2">
-        <v>6350.08</v>
+        <v>6406.52</v>
       </c>
       <c r="E8" s="2">
-        <v>1649.92</v>
+        <v>1593.48</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
@@ -569,7 +569,7 @@
       </c>
       <c r="G8" s="2">
         <f>($D$2-SUM($D$5:D7))*30/100/12</f>
-        <v>1649.9219999999998</v>
+        <v>1593.4814999999999</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="1"/>
@@ -577,7 +577,7 @@
       </c>
       <c r="K8" s="2">
         <f>($D$2-SUM($D$5:D11))*30/100/12</f>
-        <v>1331.7949999999996</v>
+        <v>822.76174999999967</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -588,18 +588,23 @@
         <v>5</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="2"/>
-        <v>53271.799999999988</v>
+        <f>C8-D9</f>
+        <v>49766.05999999999</v>
       </c>
       <c r="D9" s="2">
-        <v>6375</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>7566.68</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1433.32</v>
+      </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>6375</v>
-      </c>
-      <c r="G9" s="2"/>
+        <v>9000</v>
+      </c>
+      <c r="G9" s="2">
+        <f>($D$2-SUM($D$5:D8))*30/100/12</f>
+        <v>1433.3184999999996</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -608,13 +613,24 @@
       <c r="B10">
         <v>6</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="2">
+        <f>C9-D10</f>
+        <v>36010.209999999992</v>
+      </c>
+      <c r="D10" s="2">
+        <v>13755.85</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1244.1500000000001</v>
+      </c>
       <c r="F10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="2"/>
+        <f>D10+E10</f>
+        <v>15000</v>
+      </c>
+      <c r="G10" s="2">
+        <f>($D$2-SUM($D$5:D9))*30/100/12</f>
+        <v>1244.1514999999997</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -623,13 +639,24 @@
       <c r="B11">
         <v>7</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="2">
+        <f t="shared" ref="C11:C13" si="3">C10-D11</f>
+        <v>32910.469999999994</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3099.74</v>
+      </c>
+      <c r="E11" s="2">
+        <v>900.26</v>
+      </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="2"/>
+        <v>4000</v>
+      </c>
+      <c r="G11" s="2">
+        <f>($D$2-SUM($D$5:D10))*30/100/12</f>
+        <v>900.25524999999982</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -638,13 +665,22 @@
       <c r="B12">
         <v>8</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="C12" s="2">
+        <f t="shared" si="3"/>
+        <v>28910.469999999994</v>
+      </c>
+      <c r="D12" s="2">
+        <v>4000</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="2"/>
+        <v>4000</v>
+      </c>
+      <c r="G12" s="2">
+        <f>($D$2-SUM($D$5:D13))*30/100/12</f>
+        <v>572.76174999999967</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -653,11 +689,17 @@
       <c r="B13">
         <v>9</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="C13" s="2">
+        <f t="shared" si="3"/>
+        <v>22910.469999999994</v>
+      </c>
+      <c r="D13" s="2">
+        <v>6000</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="G13" s="2"/>
     </row>
@@ -687,31 +729,31 @@
       </c>
       <c r="D15" s="2">
         <f>SUM(D5:D14)</f>
-        <v>99728.200000000012</v>
+        <v>130089.53000000001</v>
       </c>
       <c r="E15" s="2">
         <f>SUM(E5:E14)</f>
-        <v>12646.800000000001</v>
+        <v>13910.47</v>
       </c>
       <c r="F15" s="2">
         <f>SUM(F5:F14)</f>
-        <v>112375</v>
+        <v>144000</v>
       </c>
       <c r="G15" s="2">
         <f>SUM(G5:G14)</f>
-        <v>10389.1875</v>
+        <v>14483.233999999999</v>
       </c>
       <c r="H15" s="2">
         <f>G15-E15</f>
-        <v>-2257.6125000000011</v>
+        <v>572.76399999999921</v>
       </c>
       <c r="I15" s="2">
         <f>G15+K5</f>
-        <v>11880.3575</v>
+        <v>15916.552499999998</v>
       </c>
       <c r="L15" s="2">
         <f>C8*30/100/12</f>
-        <v>1491.1699999999994</v>
+        <v>1433.3184999999996</v>
       </c>
     </row>
   </sheetData>
@@ -724,7 +766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Recambios parciales a interes periodo
</commit_message>
<xml_diff>
--- a/Calculos.xlsx
+++ b/Calculos.xlsx
@@ -24,8 +24,34 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>DevMax</author>
+  </authors>
+  <commentList>
+    <comment ref="I4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">El interes periodo se activa a partir del dia de concesion, las siguientes activaciones inicia a partir de la fehca 02/04/2021
+y ser reactivarancada mes hasta la fecha de finalizacion del credito
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Pagos</t>
   </si>
@@ -67,6 +93,27 @@
   </si>
   <si>
     <t xml:space="preserve">Deuda </t>
+  </si>
+  <si>
+    <t>Fechas esperada de pago</t>
+  </si>
+  <si>
+    <t>Interes  periodo esperado</t>
+  </si>
+  <si>
+    <t>Fecha de pago realizada</t>
+  </si>
+  <si>
+    <t>Sin pago</t>
+  </si>
+  <si>
+    <t>Saldo despues de pago</t>
+  </si>
+  <si>
+    <t>sin pago</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -76,7 +123,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$Q-100A]#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,16 +131,84 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9797"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -101,20 +216,446 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9797"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -388,377 +929,475 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B2" sqref="B2:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="F2" s="5">
         <v>153000</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="H2" s="6">
         <v>30</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2">
+      <c r="J2" s="7">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
+        <v>44257</v>
+      </c>
+      <c r="C5" s="12">
+        <v>44256</v>
+      </c>
+      <c r="D5" s="17">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8">
+        <f>$F$2-F5</f>
+        <v>116825</v>
+      </c>
+      <c r="F5" s="31">
+        <v>36175</v>
+      </c>
+      <c r="G5" s="31">
+        <v>3825</v>
+      </c>
+      <c r="H5" s="31">
+        <f>F5+G5</f>
+        <v>40000</v>
+      </c>
+      <c r="I5" s="32">
+        <f>F2*30/100/12</f>
+        <v>3825</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12">
+        <v>44277</v>
+      </c>
+      <c r="D6" s="17">
+        <v>2</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" ref="E6:E13" si="0">E5-F6</f>
+        <v>79745.62</v>
+      </c>
+      <c r="F6" s="31">
+        <v>37079.379999999997</v>
+      </c>
+      <c r="G6" s="31">
+        <v>2920.62</v>
+      </c>
+      <c r="H6" s="31">
+        <f>F6+G6</f>
+        <v>40000</v>
+      </c>
+      <c r="I6" s="32">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="13">
+        <v>44288</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="18">
+        <v>3</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="0"/>
+        <v>79745.62</v>
+      </c>
+      <c r="F7" s="33">
+        <v>0</v>
+      </c>
+      <c r="G7" s="33">
+        <v>0</v>
+      </c>
+      <c r="H7" s="33">
+        <v>0</v>
+      </c>
+      <c r="I7" s="34">
+        <f>($F$2-SUM($F$5:F6))*30/100/12</f>
+        <v>1993.6404999999997</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="11">
+        <v>44318</v>
+      </c>
+      <c r="C8" s="12">
+        <v>44320</v>
+      </c>
+      <c r="D8" s="17">
+        <v>4</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>63739.259999999995</v>
+      </c>
+      <c r="F8" s="31">
+        <v>16006.36</v>
+      </c>
+      <c r="G8" s="31">
+        <v>1993.64</v>
+      </c>
+      <c r="H8" s="31">
+        <f t="shared" ref="H8:H16" si="1">F8+G8</f>
+        <v>18000</v>
+      </c>
+      <c r="I8" s="32">
+        <f>($F$2-SUM($F$5:F7))*30/100/12</f>
+        <v>1993.6404999999997</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="11"/>
+      <c r="C9" s="12">
+        <v>44347</v>
+      </c>
+      <c r="D9" s="17">
+        <v>5</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>57332.739999999991</v>
+      </c>
+      <c r="F9" s="31">
+        <v>6406.52</v>
+      </c>
+      <c r="G9" s="31">
+        <v>1593.48</v>
+      </c>
+      <c r="H9" s="31">
+        <f>F9+G9</f>
+        <v>8000</v>
+      </c>
+      <c r="I9" s="32">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="13">
+        <v>44349</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="18">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E10" s="9">
+        <f t="shared" si="0"/>
+        <v>57332.739999999991</v>
+      </c>
+      <c r="F10" s="35">
+        <v>0</v>
+      </c>
+      <c r="G10" s="35">
+        <v>0</v>
+      </c>
+      <c r="H10" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="34">
+        <f>($F$2-SUM($F$5:F9))*30/100/12</f>
+        <v>1433.3184999999996</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="11">
+        <v>44379</v>
+      </c>
+      <c r="C11" s="12">
+        <v>44381</v>
+      </c>
+      <c r="D11" s="17">
+        <v>7</v>
+      </c>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
+        <v>49766.05999999999</v>
+      </c>
+      <c r="F11" s="31">
+        <v>7566.68</v>
+      </c>
+      <c r="G11" s="31">
+        <v>1433.32</v>
+      </c>
+      <c r="H11" s="31">
+        <f t="shared" si="1"/>
+        <v>9000</v>
+      </c>
+      <c r="I11" s="32">
+        <f>($F$2-SUM($F$5:F10))*30/100/12</f>
+        <v>1433.3184999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="11"/>
+      <c r="C12" s="12">
+        <v>44403</v>
+      </c>
+      <c r="D12" s="17">
+        <v>8</v>
+      </c>
+      <c r="E12" s="8">
+        <f t="shared" si="0"/>
+        <v>36010.209999999992</v>
+      </c>
+      <c r="F12" s="31">
+        <v>13755.85</v>
+      </c>
+      <c r="G12" s="31">
+        <v>1244.1500000000001</v>
+      </c>
+      <c r="H12" s="31">
+        <f t="shared" si="1"/>
+        <v>15000</v>
+      </c>
+      <c r="I12" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="15">
+        <v>44410</v>
+      </c>
+      <c r="C13" s="16">
+        <v>44417</v>
+      </c>
+      <c r="D13" s="19">
+        <v>9</v>
+      </c>
+      <c r="E13" s="10">
+        <f t="shared" si="0"/>
+        <v>32910.469999999994</v>
+      </c>
+      <c r="F13" s="36">
+        <v>3099.74</v>
+      </c>
+      <c r="G13" s="36">
+        <v>900.26</v>
+      </c>
+      <c r="H13" s="36">
+        <f>F13+G13</f>
+        <v>4000</v>
+      </c>
+      <c r="I13" s="37">
+        <f>($F$2-SUM($F$5:F12))*30/100/12</f>
+        <v>900.25524999999982</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="15"/>
+      <c r="C14" s="16">
+        <v>44424</v>
+      </c>
+      <c r="D14" s="19">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>44257</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <f>$D$2-D5</f>
-        <v>116825</v>
-      </c>
-      <c r="D5" s="2">
-        <v>36175</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3825</v>
-      </c>
-      <c r="F5" s="2">
-        <f>D5+E5</f>
-        <v>40000</v>
-      </c>
-      <c r="G5" s="2">
-        <f>D2*30/100/12</f>
-        <v>3825</v>
-      </c>
-      <c r="J5" s="2">
-        <f>($D$2/24)</f>
-        <v>6375</v>
-      </c>
-      <c r="K5" s="2">
-        <f>($D$2-SUM($D$5:D8))*30/100/12</f>
-        <v>1433.3184999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>44288</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2">
-        <f>C5-D6</f>
-        <v>79745.62</v>
-      </c>
-      <c r="D6" s="2">
-        <v>37079.379999999997</v>
-      </c>
-      <c r="E6" s="2">
-        <v>2920.62</v>
-      </c>
-      <c r="F6" s="2">
-        <f t="shared" ref="F6:F14" si="0">D6+E6</f>
-        <v>40000</v>
-      </c>
-      <c r="G6" s="2">
-        <f>($D$2-SUM($D$5:D5))*30/100/12</f>
-        <v>2920.625</v>
-      </c>
-      <c r="J6" s="2">
-        <f t="shared" ref="J6:J8" si="1">($D$2/24)</f>
-        <v>6375</v>
-      </c>
-      <c r="K6" s="2">
-        <f>($D$2-SUM($D$5:D9))*30/100/12</f>
-        <v>1244.1514999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>44318</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2">
-        <f t="shared" ref="C7:C9" si="2">C6-D7</f>
-        <v>63739.259999999995</v>
-      </c>
-      <c r="D7" s="2">
-        <v>16006.36</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1993.64</v>
-      </c>
-      <c r="F7" s="2">
-        <f t="shared" si="0"/>
-        <v>18000</v>
-      </c>
-      <c r="G7" s="2">
-        <f>($D$2-SUM($D$5:D6))*30/100/12</f>
-        <v>1993.6404999999997</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="E14" s="10">
+        <f t="shared" ref="E14:E15" si="2">E13-F14</f>
+        <v>28910.469999999994</v>
+      </c>
+      <c r="F14" s="36">
+        <v>4000</v>
+      </c>
+      <c r="G14" s="36">
+        <v>0</v>
+      </c>
+      <c r="H14" s="36">
+        <f>F14+G14</f>
+        <v>4000</v>
+      </c>
+      <c r="I14" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="15"/>
+      <c r="C15" s="16">
+        <v>44439</v>
+      </c>
+      <c r="D15" s="19">
+        <v>11</v>
+      </c>
+      <c r="E15" s="10">
+        <f t="shared" si="2"/>
+        <v>22910.469999999994</v>
+      </c>
+      <c r="F15" s="36">
+        <v>6000</v>
+      </c>
+      <c r="G15" s="36">
+        <v>0</v>
+      </c>
+      <c r="H15" s="36"/>
+      <c r="I15" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="27">
+        <v>44441</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="29">
+        <v>12</v>
+      </c>
+      <c r="E16" s="30">
+        <f>E13-F16</f>
+        <v>32910.469999999994</v>
+      </c>
+      <c r="F16" s="38">
+        <v>0</v>
+      </c>
+      <c r="G16" s="38">
+        <v>0</v>
+      </c>
+      <c r="H16" s="38">
         <f t="shared" si="1"/>
-        <v>6375</v>
-      </c>
-      <c r="K7" s="2">
-        <f>($D$2-SUM($D$5:D10))*30/100/12</f>
-        <v>900.25524999999982</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>44349</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2">
-        <f t="shared" si="2"/>
-        <v>57332.739999999991</v>
-      </c>
-      <c r="D8" s="2">
-        <v>6406.52</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1593.48</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="0"/>
-        <v>8000</v>
-      </c>
-      <c r="G8" s="2">
-        <f>($D$2-SUM($D$5:D7))*30/100/12</f>
-        <v>1593.4814999999999</v>
-      </c>
-      <c r="J8" s="2">
-        <f t="shared" si="1"/>
-        <v>6375</v>
-      </c>
-      <c r="K8" s="2">
-        <f>($D$2-SUM($D$5:D11))*30/100/12</f>
-        <v>822.76174999999967</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>44379</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2">
-        <f>C8-D9</f>
-        <v>49766.05999999999</v>
-      </c>
-      <c r="D9" s="2">
-        <v>7566.68</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1433.32</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="0"/>
-        <v>9000</v>
-      </c>
-      <c r="G9" s="2">
-        <f>($D$2-SUM($D$5:D8))*30/100/12</f>
-        <v>1433.3184999999996</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>44410</v>
-      </c>
-      <c r="B10">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2">
-        <f>C9-D10</f>
-        <v>36010.209999999992</v>
-      </c>
-      <c r="D10" s="2">
-        <v>13755.85</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1244.1500000000001</v>
-      </c>
-      <c r="F10" s="2">
-        <f>D10+E10</f>
-        <v>15000</v>
-      </c>
-      <c r="G10" s="2">
-        <f>($D$2-SUM($D$5:D9))*30/100/12</f>
-        <v>1244.1514999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>44441</v>
-      </c>
-      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="I16" s="39">
+        <f>($F$2-SUM($F$5:F15))*30/100/12</f>
+        <v>572.76174999999967</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2">
-        <f t="shared" ref="C11:C13" si="3">C10-D11</f>
-        <v>32910.469999999994</v>
-      </c>
-      <c r="D11" s="2">
-        <v>3099.74</v>
-      </c>
-      <c r="E11" s="2">
-        <v>900.26</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-      <c r="G11" s="2">
-        <f>($D$2-SUM($D$5:D10))*30/100/12</f>
-        <v>900.25524999999982</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>44471</v>
-      </c>
-      <c r="B12">
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="46">
+        <f ca="1">SUM(F5:F17)</f>
+        <v>130089.53000000001</v>
+      </c>
+      <c r="G17" s="48">
+        <f ca="1">SUM(G5:G17)</f>
+        <v>13910.47</v>
+      </c>
+      <c r="H17" s="48">
+        <f ca="1">SUM(H5:H17)</f>
+        <v>138000</v>
+      </c>
+      <c r="I17" s="50">
+        <f ca="1">SUM(I5:I17)</f>
+        <v>12151.934999999998</v>
+      </c>
+      <c r="J17" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2">
-        <f t="shared" si="3"/>
-        <v>28910.469999999994</v>
-      </c>
-      <c r="D12" s="2">
-        <v>4000</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2">
-        <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-      <c r="G12" s="2">
-        <f>($D$2-SUM($D$5:D13))*30/100/12</f>
-        <v>572.76174999999967</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>44502</v>
-      </c>
-      <c r="B13">
+      <c r="K17" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2">
-        <f t="shared" si="3"/>
-        <v>22910.469999999994</v>
-      </c>
-      <c r="D13" s="2">
-        <v>6000</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2">
-        <f t="shared" si="0"/>
-        <v>6000</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>44532</v>
-      </c>
-      <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="2">
-        <f>SUM(D5:D14)</f>
-        <v>130089.53000000001</v>
-      </c>
-      <c r="E15" s="2">
-        <f>SUM(E5:E14)</f>
-        <v>13910.47</v>
-      </c>
-      <c r="F15" s="2">
-        <f>SUM(F5:F14)</f>
-        <v>144000</v>
-      </c>
-      <c r="G15" s="2">
-        <f>SUM(G5:G14)</f>
-        <v>14483.233999999999</v>
-      </c>
-      <c r="H15" s="2">
-        <f>G15-E15</f>
-        <v>572.76399999999921</v>
-      </c>
-      <c r="I15" s="2">
-        <f>G15+K5</f>
-        <v>15916.552499999998</v>
-      </c>
-      <c r="L15" s="2">
-        <f>C8*30/100/12</f>
-        <v>1433.3184999999996</v>
-      </c>
+    </row>
+    <row r="18" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="43"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="25">
+        <f ca="1">I17-G17</f>
+        <v>-1758.5350000000017</v>
+      </c>
+      <c r="K18" s="26">
+        <f ca="1">I17+M5</f>
+        <v>12151.934999999998</v>
+      </c>
+      <c r="N18" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="4294967293" verticalDpi="203" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>